<commit_message>
feat: rebuild Excel fixtures and make parser Excel-only
</commit_message>
<xml_diff>
--- a/data/test-files/no_queries.xlsx
+++ b/data/test-files/no_queries.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
feat: add Power BI (.pbix/.pbit) file ingestion support
Add parsePbixFile() that reads the DataMashup binary directly from the
root of Power BI ZIP archives (unlike .xlsx where it is embedded in
customXml). Both .pbix and .pbit files use the same MS-QDEFF format
that the existing extractFromDataMashup() already handles, so the
inner parsing pipeline is fully reused.

Changes:
- power-query-explorer.html: new parsePbixFile(), isPbixFile(),
  isSupportedFile() helpers; updated file filters, drop zone UI,
  accept attribute, and limitations text
- scripts/create_test_files.py: new create_pbix_file() builder and
  three test fixtures (simple_query.pbix, multi_query.pbix,
  simple_query.pbit)
- scripts/test_explorer.py: four new Playwright tests for .pbix,
  .pbit, and mixed .xlsx+.pbix uploads
- README.md: updated to reflect .pbix/.pbit support

https://claude.ai/code/session_01M1RifGG1zk6pvxgtwfuPr5
</commit_message>
<xml_diff>
--- a/data/test-files/no_queries.xlsx
+++ b/data/test-files/no_queries.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>